<commit_message>
Improved error handling and logging
</commit_message>
<xml_diff>
--- a/CTX-PS-Example-Spreadsheet.xlsx
+++ b/CTX-PS-Example-Spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stephen.connor\Documents\PreSales information\Studio Packages\GitHub Clones\CTX-PS-Process-Spreadsheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7E6AD976-E890-44D6-868B-9165EAB253EB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E5E0EDA-3EC9-4F99-92B1-EB23573932CD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33945" yWindow="1050" windowWidth="20205" windowHeight="9330" xr2:uid="{EF72DB2B-479E-42E2-AD60-D8CB717E6854}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{EF72DB2B-479E-42E2-AD60-D8CB717E6854}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>CustomerId</t>
   </si>
@@ -63,9 +63,6 @@
     <t>ABC$1</t>
   </si>
   <si>
-    <t>Exxon</t>
-  </si>
-  <si>
     <t>CREATE</t>
   </si>
   <si>
@@ -79,6 +76,21 @@
   </si>
   <si>
     <t>10-March-1965</t>
+  </si>
+  <si>
+    <t>Apple</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>+155567179876</t>
+  </si>
+  <si>
+    <t>+44 2040001234</t>
+  </si>
+  <si>
+    <t>1–800–854–3680</t>
   </si>
 </sst>
 </file>
@@ -432,19 +444,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7653099E-69F4-4464-8FD9-018E8FD18AAD}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="10.7265625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.90625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -458,10 +472,13 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -472,13 +489,16 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="1">
+        <v>9</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="1">
         <v>43831</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -489,13 +509,16 @@
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>13</v>
+        <v>17</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -503,13 +526,16 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>14</v>
+        <v>18</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>